<commit_message>
Minor changes in comparator class & added description
</commit_message>
<xml_diff>
--- a/Daily WO.xlsx
+++ b/Daily WO.xlsx
@@ -73,6 +73,9 @@
     <t>UL.</t>
   </si>
   <si>
+    <t>CHEŁMOŃSKIEGO JÓZEFA</t>
+  </si>
+  <si>
     <t>KRAKÓW</t>
   </si>
   <si>
@@ -431,9 +434,6 @@
   </si>
   <si>
     <t>PROMIENISTYCH</t>
-  </si>
-  <si>
-    <t>CHEŁMONSKIEGO JÓZEFA</t>
   </si>
 </sst>
 </file>
@@ -1283,9 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1359,7 +1357,7 @@
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -1368,19 +1366,19 @@
         <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O2" s="1">
         <v>32533900</v>
       </c>
       <c r="P2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1403,7 +1401,7 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>13</v>
@@ -1412,19 +1410,19 @@
         <v>122</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O3" s="1">
         <v>32554819</v>
       </c>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1447,7 +1445,7 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4">
         <v>26</v>
@@ -1456,19 +1454,19 @@
         <v>67</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O4" s="1">
         <v>32573744</v>
       </c>
       <c r="P4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1488,13 +1486,13 @@
         <v>51323</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5">
         <v>57</v>
@@ -1503,19 +1501,19 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O5" s="1">
         <v>32576303</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1538,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -1547,19 +1545,19 @@
         <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O6" s="1">
         <v>32581440</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1582,28 +1580,28 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J7">
         <v>85</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O7" s="1">
         <v>32583159</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1626,7 +1624,7 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8">
         <v>21</v>
@@ -1635,19 +1633,19 @@
         <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O8" s="1">
         <v>32584425</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1667,13 +1665,13 @@
         <v>49727</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I9">
         <v>12</v>
@@ -1682,19 +1680,19 @@
         <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O9" s="1">
         <v>32593975</v>
       </c>
       <c r="P9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1717,7 +1715,7 @@
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I10">
         <v>23</v>
@@ -1726,13 +1724,13 @@
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N10">
         <v>124124928</v>
@@ -1741,7 +1739,7 @@
         <v>32597767</v>
       </c>
       <c r="P10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1761,13 +1759,13 @@
         <v>35799</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I11">
         <v>19</v>
@@ -1776,13 +1774,13 @@
         <v>85</v>
       </c>
       <c r="K11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N11">
         <v>124115734</v>
@@ -1791,7 +1789,7 @@
         <v>32598609</v>
       </c>
       <c r="P11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1811,13 +1809,13 @@
         <v>3340314</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I12">
         <v>32</v>
@@ -1826,19 +1824,19 @@
         <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O12" s="1">
         <v>32599213</v>
       </c>
       <c r="P12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1861,7 +1859,7 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1870,19 +1868,19 @@
         <v>47</v>
       </c>
       <c r="K13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O13" s="1">
         <v>32599294</v>
       </c>
       <c r="P13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1902,13 +1900,13 @@
         <v>3831979</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I14">
         <v>22</v>
@@ -1917,19 +1915,19 @@
         <v>21</v>
       </c>
       <c r="K14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O14" s="1">
         <v>32599980</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1952,7 +1950,7 @@
         <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I15">
         <v>14</v>
@@ -1961,13 +1959,13 @@
         <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N15">
         <v>124117474</v>
@@ -1976,7 +1974,7 @@
         <v>32601237</v>
       </c>
       <c r="P15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1996,13 +1994,13 @@
         <v>3832250</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I16">
         <v>66</v>
@@ -2011,19 +2009,19 @@
         <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O16" s="1">
         <v>32603924</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2043,34 +2041,34 @@
         <v>2653468</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J17">
         <v>10</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O17" s="1">
         <v>32605118</v>
       </c>
       <c r="P17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2090,34 +2088,34 @@
         <v>3540942</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J18">
         <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O18" s="1">
         <v>32605119</v>
       </c>
       <c r="P18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2137,13 +2135,13 @@
         <v>2331508</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I19">
         <v>8</v>
@@ -2152,19 +2150,19 @@
         <v>46</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O19" s="1">
         <v>32605183</v>
       </c>
       <c r="P19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2184,13 +2182,13 @@
         <v>1908563</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I20">
         <v>29</v>
@@ -2199,19 +2197,19 @@
         <v>37</v>
       </c>
       <c r="K20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O20" s="1">
         <v>32605710</v>
       </c>
       <c r="P20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2231,13 +2229,13 @@
         <v>3542730</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
         <v>18</v>
       </c>
       <c r="H21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I21">
         <v>16</v>
@@ -2246,19 +2244,19 @@
         <v>55</v>
       </c>
       <c r="K21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O21" s="1">
         <v>32606082</v>
       </c>
       <c r="P21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2278,13 +2276,13 @@
         <v>3807812</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
       </c>
       <c r="H22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -2293,19 +2291,19 @@
         <v>100</v>
       </c>
       <c r="K22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O22" s="1">
         <v>32606947</v>
       </c>
       <c r="P22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2328,7 +2326,7 @@
         <v>18</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I23">
         <v>4</v>
@@ -2337,19 +2335,19 @@
         <v>53</v>
       </c>
       <c r="K23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O23" s="1">
         <v>32607315</v>
       </c>
       <c r="P23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -2372,28 +2370,28 @@
         <v>18</v>
       </c>
       <c r="H24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O24" s="1">
         <v>32607474</v>
       </c>
       <c r="P24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2416,7 +2414,7 @@
         <v>18</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I25">
         <v>14</v>
@@ -2425,19 +2423,19 @@
         <v>11</v>
       </c>
       <c r="K25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O25" s="1">
         <v>32607981</v>
       </c>
       <c r="P25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2457,13 +2455,13 @@
         <v>47341</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I26">
         <v>10</v>
@@ -2472,13 +2470,13 @@
         <v>11</v>
       </c>
       <c r="K26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N26">
         <v>124118176</v>
@@ -2487,7 +2485,7 @@
         <v>32615613</v>
       </c>
       <c r="P26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2513,7 +2511,7 @@
         <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I27">
         <v>14</v>
@@ -2522,19 +2520,19 @@
         <v>2</v>
       </c>
       <c r="K27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O27" s="1">
         <v>32615672</v>
       </c>
       <c r="P27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -2560,7 +2558,7 @@
         <v>18</v>
       </c>
       <c r="H28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I28">
         <v>18</v>
@@ -2569,19 +2567,19 @@
         <v>85</v>
       </c>
       <c r="K28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O28" s="1">
         <v>32615847</v>
       </c>
       <c r="P28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2601,13 +2599,13 @@
         <v>3832538</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G29" t="s">
         <v>18</v>
       </c>
       <c r="H29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I29">
         <v>24</v>
@@ -2616,19 +2614,19 @@
         <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O29" s="1">
         <v>32615885</v>
       </c>
       <c r="P29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2648,13 +2646,13 @@
         <v>3832542</v>
       </c>
       <c r="F30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G30" t="s">
         <v>18</v>
       </c>
       <c r="H30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I30">
         <v>24</v>
@@ -2663,19 +2661,19 @@
         <v>22</v>
       </c>
       <c r="K30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O30" s="1">
         <v>32616195</v>
       </c>
       <c r="P30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2698,7 +2696,7 @@
         <v>18</v>
       </c>
       <c r="H31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I31">
         <v>104</v>
@@ -2707,19 +2705,19 @@
         <v>23</v>
       </c>
       <c r="K31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O31" s="1">
         <v>32616349</v>
       </c>
       <c r="P31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -2739,34 +2737,34 @@
         <v>2631779</v>
       </c>
       <c r="F32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J32">
         <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O32" s="1">
         <v>32616400</v>
       </c>
       <c r="P32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2786,13 +2784,13 @@
         <v>3832569</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G33" t="s">
         <v>18</v>
       </c>
       <c r="H33" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I33">
         <v>12</v>
@@ -2801,19 +2799,19 @@
         <v>24</v>
       </c>
       <c r="K33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O33" s="1">
         <v>32617072</v>
       </c>
       <c r="P33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -2836,7 +2834,7 @@
         <v>18</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I34">
         <v>20</v>
@@ -2845,13 +2843,13 @@
         <v>58</v>
       </c>
       <c r="K34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N34">
         <v>124239138</v>
@@ -2860,7 +2858,7 @@
         <v>32617538</v>
       </c>
       <c r="P34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2883,7 +2881,7 @@
         <v>18</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I35">
         <v>18</v>
@@ -2892,19 +2890,19 @@
         <v>21</v>
       </c>
       <c r="K35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O35" s="1">
         <v>32617556</v>
       </c>
       <c r="P35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2924,10 +2922,10 @@
         <v>3089202</v>
       </c>
       <c r="G36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I36">
         <v>31</v>
@@ -2936,13 +2934,13 @@
         <v>14</v>
       </c>
       <c r="K36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L36" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M36" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N36">
         <v>123521552</v>
@@ -2951,7 +2949,7 @@
         <v>32617575</v>
       </c>
       <c r="P36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -2974,7 +2972,7 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I37">
         <v>2</v>
@@ -2983,19 +2981,19 @@
         <v>11</v>
       </c>
       <c r="K37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L37" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O37" s="1">
         <v>32617928</v>
       </c>
       <c r="P37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3018,7 +3016,7 @@
         <v>18</v>
       </c>
       <c r="H38" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I38">
         <v>19</v>
@@ -3027,13 +3025,13 @@
         <v>17</v>
       </c>
       <c r="K38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N38">
         <v>124123172</v>
@@ -3042,7 +3040,7 @@
         <v>32618171</v>
       </c>
       <c r="P38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3062,13 +3060,13 @@
         <v>2213814</v>
       </c>
       <c r="F39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G39" t="s">
         <v>18</v>
       </c>
       <c r="H39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I39">
         <v>9</v>
@@ -3077,13 +3075,13 @@
         <v>98</v>
       </c>
       <c r="K39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L39" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M39" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N39">
         <v>123112996</v>
@@ -3092,7 +3090,7 @@
         <v>32618632</v>
       </c>
       <c r="P39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3115,7 +3113,7 @@
         <v>18</v>
       </c>
       <c r="H40" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I40">
         <v>26</v>
@@ -3124,13 +3122,13 @@
         <v>19</v>
       </c>
       <c r="K40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N40">
         <v>124226780</v>
@@ -3139,7 +3137,7 @@
         <v>32619044</v>
       </c>
       <c r="P40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3159,34 +3157,34 @@
         <v>3479679</v>
       </c>
       <c r="F41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G41" t="s">
         <v>18</v>
       </c>
       <c r="H41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I41" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J41">
         <v>42</v>
       </c>
       <c r="K41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L41" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M41" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O41" s="1">
         <v>32619514</v>
       </c>
       <c r="P41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3209,7 +3207,7 @@
         <v>18</v>
       </c>
       <c r="H42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I42">
         <v>12</v>
@@ -3218,13 +3216,13 @@
         <v>61</v>
       </c>
       <c r="K42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L42" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M42" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N42">
         <v>124111162</v>
@@ -3233,7 +3231,7 @@
         <v>32619733</v>
       </c>
       <c r="P42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3256,7 +3254,7 @@
         <v>18</v>
       </c>
       <c r="H43" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I43">
         <v>15</v>
@@ -3265,19 +3263,19 @@
         <v>27</v>
       </c>
       <c r="K43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M43" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O43" s="1">
         <v>32620944</v>
       </c>
       <c r="P43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3297,13 +3295,13 @@
         <v>3832226</v>
       </c>
       <c r="F44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I44">
         <v>3</v>
@@ -3312,19 +3310,19 @@
         <v>14</v>
       </c>
       <c r="K44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O44" s="1">
         <v>32621709</v>
       </c>
       <c r="P44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3344,13 +3342,13 @@
         <v>3537511</v>
       </c>
       <c r="F45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G45" t="s">
         <v>18</v>
       </c>
       <c r="H45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I45">
         <v>19</v>
@@ -3359,19 +3357,19 @@
         <v>10</v>
       </c>
       <c r="K45" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O45" s="1">
         <v>32622665</v>
       </c>
       <c r="P45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3391,13 +3389,13 @@
         <v>3832734</v>
       </c>
       <c r="F46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G46" t="s">
         <v>18</v>
       </c>
       <c r="H46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I46">
         <v>5</v>
@@ -3406,19 +3404,19 @@
         <v>88</v>
       </c>
       <c r="K46" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L46" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M46" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O46" s="1">
         <v>32623354</v>
       </c>
       <c r="P46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3441,7 +3439,7 @@
         <v>18</v>
       </c>
       <c r="H47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I47">
         <v>122</v>
@@ -3450,19 +3448,19 @@
         <v>63</v>
       </c>
       <c r="K47" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O47" s="1">
         <v>32623362</v>
       </c>
       <c r="P47" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3485,7 +3483,7 @@
         <v>18</v>
       </c>
       <c r="H48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I48">
         <v>14</v>
@@ -3494,19 +3492,19 @@
         <v>29</v>
       </c>
       <c r="K48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O48" s="1">
         <v>32623990</v>
       </c>
       <c r="P48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3526,13 +3524,13 @@
         <v>3673304</v>
       </c>
       <c r="F49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G49" t="s">
         <v>18</v>
       </c>
       <c r="H49" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I49">
         <v>14</v>
@@ -3541,19 +3539,19 @@
         <v>40</v>
       </c>
       <c r="K49" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L49" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M49" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O49" s="1">
         <v>32624016</v>
       </c>
       <c r="P49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3573,13 +3571,13 @@
         <v>3673304</v>
       </c>
       <c r="F50" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G50" t="s">
         <v>18</v>
       </c>
       <c r="H50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I50">
         <v>8</v>
@@ -3588,19 +3586,19 @@
         <v>38</v>
       </c>
       <c r="K50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L50" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M50" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O50" s="1">
         <v>32624033</v>
       </c>
       <c r="P50" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3620,13 +3618,13 @@
         <v>3784682</v>
       </c>
       <c r="F51" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G51" t="s">
         <v>18</v>
       </c>
       <c r="H51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I51">
         <v>3</v>
@@ -3635,19 +3633,19 @@
         <v>25</v>
       </c>
       <c r="K51" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L51" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M51" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O51" s="1">
         <v>32624170</v>
       </c>
       <c r="P51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -3670,22 +3668,22 @@
         <v>18</v>
       </c>
       <c r="H52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I52" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J52">
         <v>23</v>
       </c>
       <c r="K52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L52" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M52" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N52">
         <v>124152751</v>
@@ -3694,7 +3692,7 @@
         <v>32624802</v>
       </c>
       <c r="P52" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -3714,13 +3712,13 @@
         <v>3808445</v>
       </c>
       <c r="F53" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G53" t="s">
         <v>18</v>
       </c>
       <c r="H53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I53">
         <v>5</v>
@@ -3729,19 +3727,19 @@
         <v>46</v>
       </c>
       <c r="K53" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L53" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M53" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O53" s="1">
         <v>32625661</v>
       </c>
       <c r="P53" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -3764,28 +3762,28 @@
         <v>18</v>
       </c>
       <c r="H54" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J54">
         <v>114</v>
       </c>
       <c r="K54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L54" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M54" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O54" s="1">
         <v>32625981</v>
       </c>
       <c r="P54" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -3805,34 +3803,34 @@
         <v>3372711</v>
       </c>
       <c r="F55" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G55" t="s">
         <v>18</v>
       </c>
       <c r="H55" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I55" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J55">
         <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L55" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M55" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O55" s="1">
         <v>32628152</v>
       </c>
       <c r="P55" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -3852,13 +3850,13 @@
         <v>30770</v>
       </c>
       <c r="F56" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G56" t="s">
         <v>18</v>
       </c>
       <c r="H56" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I56">
         <v>48</v>
@@ -3867,13 +3865,13 @@
         <v>32</v>
       </c>
       <c r="K56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M56" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N56">
         <v>123588904</v>
@@ -3882,7 +3880,7 @@
         <v>32628476</v>
       </c>
       <c r="P56" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -3902,31 +3900,31 @@
         <v>2880962</v>
       </c>
       <c r="G57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H57" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J57">
         <v>16</v>
       </c>
       <c r="K57" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L57" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M57" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O57" s="1">
         <v>32628576</v>
       </c>
       <c r="P57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -3949,7 +3947,7 @@
         <v>18</v>
       </c>
       <c r="H58" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I58">
         <v>13</v>
@@ -3958,19 +3956,19 @@
         <v>16</v>
       </c>
       <c r="K58" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L58" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M58" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O58" s="1">
         <v>32629038</v>
       </c>
       <c r="P58" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -3990,13 +3988,13 @@
         <v>21452</v>
       </c>
       <c r="F59" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G59" t="s">
         <v>18</v>
       </c>
       <c r="H59" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I59">
         <v>5</v>
@@ -4005,13 +4003,13 @@
         <v>40</v>
       </c>
       <c r="K59" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L59" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M59" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N59">
         <v>124110278</v>
@@ -4020,7 +4018,7 @@
         <v>32629608</v>
       </c>
       <c r="P59" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -4040,34 +4038,34 @@
         <v>2261606</v>
       </c>
       <c r="F60" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G60" t="s">
         <v>18</v>
       </c>
       <c r="H60" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J60">
         <v>53</v>
       </c>
       <c r="K60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M60" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O60" s="1">
         <v>32629701</v>
       </c>
       <c r="P60" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -4087,28 +4085,28 @@
         <v>291506</v>
       </c>
       <c r="F61" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G61" t="s">
         <v>18</v>
       </c>
       <c r="H61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I61" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J61">
         <v>35</v>
       </c>
       <c r="K61" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L61" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M61" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N61">
         <v>124154607</v>
@@ -4117,7 +4115,7 @@
         <v>32630057</v>
       </c>
       <c r="P61" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -4140,28 +4138,28 @@
         <v>18</v>
       </c>
       <c r="H62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I62" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J62">
         <v>47</v>
       </c>
       <c r="K62" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L62" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M62" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O62" s="1">
         <v>32630211</v>
       </c>
       <c r="P62" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -4184,7 +4182,7 @@
         <v>18</v>
       </c>
       <c r="H63" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I63">
         <v>20</v>
@@ -4193,19 +4191,19 @@
         <v>85</v>
       </c>
       <c r="K63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L63" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M63" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O63" s="1">
         <v>32630351</v>
       </c>
       <c r="P63" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -4228,28 +4226,28 @@
         <v>18</v>
       </c>
       <c r="H64" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I64" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J64">
         <v>35</v>
       </c>
       <c r="K64" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L64" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M64" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O64" s="1">
         <v>32630778</v>
       </c>
       <c r="P64" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -4269,13 +4267,13 @@
         <v>3470393</v>
       </c>
       <c r="F65" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G65" t="s">
         <v>18</v>
       </c>
       <c r="H65" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I65">
         <v>17</v>
@@ -4284,19 +4282,19 @@
         <v>11</v>
       </c>
       <c r="K65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O65" s="1">
         <v>32631017</v>
       </c>
       <c r="P65" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -4319,7 +4317,7 @@
         <v>18</v>
       </c>
       <c r="H66" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I66">
         <v>4</v>
@@ -4328,19 +4326,19 @@
         <v>72</v>
       </c>
       <c r="K66" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L66" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O66" s="1">
         <v>32631033</v>
       </c>
       <c r="P66" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -4360,13 +4358,13 @@
         <v>3543157</v>
       </c>
       <c r="F67" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G67" t="s">
         <v>18</v>
       </c>
       <c r="H67" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I67">
         <v>14</v>
@@ -4375,19 +4373,19 @@
         <v>2</v>
       </c>
       <c r="K67" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L67" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M67" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O67" s="1">
         <v>32631422</v>
       </c>
       <c r="P67" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -4410,28 +4408,28 @@
         <v>18</v>
       </c>
       <c r="H68" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I68" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J68">
         <v>286</v>
       </c>
       <c r="K68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L68" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M68" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O68" s="1">
         <v>32631621</v>
       </c>
       <c r="P68" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -4451,13 +4449,13 @@
         <v>3644589</v>
       </c>
       <c r="F69" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G69" t="s">
         <v>18</v>
       </c>
       <c r="H69" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I69">
         <v>4</v>
@@ -4466,19 +4464,19 @@
         <v>47</v>
       </c>
       <c r="K69" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L69" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M69" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O69" s="1">
         <v>32631935</v>
       </c>
       <c r="P69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -4498,34 +4496,34 @@
         <v>3671757</v>
       </c>
       <c r="F70" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G70" t="s">
         <v>18</v>
       </c>
       <c r="H70" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I70" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J70">
         <v>23</v>
       </c>
       <c r="K70" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L70" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M70" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O70" s="1">
         <v>32632177</v>
       </c>
       <c r="P70" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -4548,28 +4546,28 @@
         <v>18</v>
       </c>
       <c r="H71" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I71" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J71">
         <v>58</v>
       </c>
       <c r="K71" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L71" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M71" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O71" s="1">
         <v>32632348</v>
       </c>
       <c r="P71" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -4589,13 +4587,13 @@
         <v>40062</v>
       </c>
       <c r="F72" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G72" t="s">
         <v>18</v>
       </c>
       <c r="H72" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I72">
         <v>4</v>
@@ -4604,13 +4602,13 @@
         <v>7</v>
       </c>
       <c r="K72" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L72" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M72" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N72">
         <v>124172599</v>
@@ -4619,7 +4617,7 @@
         <v>32632551</v>
       </c>
       <c r="P72" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -4639,13 +4637,13 @@
         <v>38051</v>
       </c>
       <c r="F73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G73" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H73" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I73">
         <v>29</v>
@@ -4654,13 +4652,13 @@
         <v>11</v>
       </c>
       <c r="K73" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M73" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N73">
         <v>124131398</v>
@@ -4669,7 +4667,7 @@
         <v>32632721</v>
       </c>
       <c r="P73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -4689,13 +4687,13 @@
         <v>23333</v>
       </c>
       <c r="F74" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G74" t="s">
         <v>18</v>
       </c>
       <c r="H74" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I74">
         <v>2</v>
@@ -4704,13 +4702,13 @@
         <v>35</v>
       </c>
       <c r="K74" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M74" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N74">
         <v>124127721</v>
@@ -4719,7 +4717,7 @@
         <v>32633546</v>
       </c>
       <c r="P74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -4739,13 +4737,13 @@
         <v>2837356</v>
       </c>
       <c r="F75" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G75" t="s">
         <v>18</v>
       </c>
       <c r="H75" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I75">
         <v>15</v>
@@ -4754,19 +4752,19 @@
         <v>105</v>
       </c>
       <c r="K75" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L75" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M75" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O75" s="1">
         <v>32634074</v>
       </c>
       <c r="P75" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -4789,7 +4787,7 @@
         <v>18</v>
       </c>
       <c r="H76" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I76">
         <v>25</v>
@@ -4798,19 +4796,19 @@
         <v>4</v>
       </c>
       <c r="K76" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L76" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M76" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O76" s="1">
         <v>32634828</v>
       </c>
       <c r="P76" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -4830,13 +4828,13 @@
         <v>3805069</v>
       </c>
       <c r="F77" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G77" t="s">
         <v>18</v>
       </c>
       <c r="H77" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I77">
         <v>11</v>
@@ -4845,19 +4843,19 @@
         <v>44</v>
       </c>
       <c r="K77" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L77" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M77" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O77" s="1">
         <v>32635083</v>
       </c>
       <c r="P77" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>